<commit_message>
GHS-1 changed dietary assessment category in DPE
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_GHS_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_GHS_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A14A4A-3C42-4983-BFAA-6FA3F437256F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{8C18C908-9092-4FA1-8769-04F00D2E3926}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1036,9 +1036,6 @@
     <t>paste</t>
   </si>
   <si>
-    <t>1 (FFQ)</t>
-  </si>
-  <si>
     <t>identical</t>
   </si>
   <si>
@@ -1070,6 +1067,9 @@
   </si>
   <si>
     <t>qu_nutr_potato_c;qu_nutr_fries_c</t>
+  </si>
+  <si>
+    <t>0 (FFQ)</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1498,7 @@
   <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F102" sqref="F102"/>
+      <selection activeCell="I121" sqref="I121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
         <v>253</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>256</v>
@@ -1597,7 +1597,7 @@
         <v>253</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>256</v>
@@ -2270,7 +2270,7 @@
         <v>256</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>272</v>
@@ -4534,7 +4534,7 @@
         <v>321</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J95" s="3" t="s">
         <v>322</v>
@@ -4598,7 +4598,7 @@
         <v>326</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J97" s="3" t="s">
         <v>322</v>
@@ -4631,7 +4631,7 @@
         <v>328</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J98" s="3" t="s">
         <v>322</v>
@@ -4726,7 +4726,7 @@
         <v>329</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J101" s="3" t="s">
         <v>322</v>
@@ -5345,16 +5345,16 @@
         <v>333</v>
       </c>
       <c r="H121" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="J121" s="3" t="s">
         <v>322</v>
       </c>
       <c r="K121" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="L121" s="3"/>
     </row>

</xml_diff>

<commit_message>
GHS-1 forgot to change respective comment in line 121 - done now
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_GHS_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_GHS_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{8C18C908-9092-4FA1-8769-04F00D2E3926}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{46533E73-D954-48BE-8D60-1B0D967FBA9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1069,7 +1069,7 @@
     <t>qu_nutr_potato_c;qu_nutr_fries_c</t>
   </si>
   <si>
-    <t>0 (FFQ)</t>
+    <t>0 (FPQ)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
GHS-1 added operation as rule for VEGETABLES_02 and removed the two variables sacapi_sm019_tx and sacapi_sm020_tx in the algorithm column for ALC_BEV_14, since I decided to also leave them out of the subgroup on mixed alcoholic drinks
</commit_message>
<xml_diff>
--- a/analyst/Franzi/rmonize/data_proc_elem/DPE_GHS_FRANZI.xlsx
+++ b/analyst/Franzi/rmonize/data_proc_elem/DPE_GHS_FRANZI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\analyst\Franzi\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{46533E73-D954-48BE-8D60-1B0D967FBA9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{79180866-3050-4E6C-9DF7-03727F683D12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="342">
   <si>
     <t>index</t>
   </si>
@@ -991,9 +991,6 @@
     <t>qu_nutr_water_c</t>
   </si>
   <si>
-    <t>sacapi_sm019_i_4 + sacapi_sm020_i_4 + sacapi_sm019_i_1 + sacapi_sm020_i_1 + sacapi_sm019_i_5 + sacapi_sm020_i_5 + sacapi_sm019_i_6 + sacapi_sm019_tx + sacapi_sm020_i_6 + sacapi_sm020_tx</t>
-  </si>
-  <si>
     <t>sacapi_sm019_i_4;sacapi_sm020_i_4</t>
   </si>
   <si>
@@ -1070,6 +1067,9 @@
   </si>
   <si>
     <t>0 (FPQ)</t>
+  </si>
+  <si>
+    <t>sacapi_sm019_i_4 + sacapi_sm020_i_4 + sacapi_sm019_i_1 + sacapi_sm020_i_1 + sacapi_sm019_i_5 + sacapi_sm020_i_5 + sacapi_sm019_i_6 + sacapi_sm020_i_6</t>
   </si>
 </sst>
 </file>
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I121" sqref="I121"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,7 +1564,7 @@
         <v>253</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>256</v>
@@ -1597,7 +1597,7 @@
         <v>253</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>256</v>
@@ -1663,7 +1663,9 @@
       <c r="F5" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>256</v>
+      </c>
       <c r="H5" s="3" t="s">
         <v>260</v>
       </c>
@@ -2270,7 +2272,7 @@
         <v>256</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="I24" s="6" t="s">
         <v>272</v>
@@ -4492,22 +4494,22 @@
         <v>253</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>256</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>319</v>
+        <v>341</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J94" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="K94" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="K94" s="3" t="s">
-        <v>323</v>
       </c>
       <c r="L94" s="3"/>
     </row>
@@ -4525,22 +4527,22 @@
         <v>253</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>256</v>
       </c>
       <c r="H95" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="J95" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="I95" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="J95" s="3" t="s">
+      <c r="K95" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="K95" s="3" t="s">
-        <v>323</v>
       </c>
       <c r="L95" s="3"/>
     </row>
@@ -4589,22 +4591,22 @@
         <v>253</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>256</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J97" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="K97" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="K97" s="3" t="s">
-        <v>323</v>
       </c>
       <c r="L97" s="3"/>
     </row>
@@ -4622,22 +4624,22 @@
         <v>253</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>256</v>
       </c>
       <c r="H98" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J98" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="K98" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="K98" s="3" t="s">
-        <v>323</v>
       </c>
       <c r="L98" s="3"/>
     </row>
@@ -4717,22 +4719,22 @@
         <v>253</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>256</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J101" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="K101" s="3" t="s">
         <v>322</v>
-      </c>
-      <c r="K101" s="3" t="s">
-        <v>323</v>
       </c>
       <c r="L101" s="3"/>
     </row>
@@ -5339,22 +5341,22 @@
         <v>253</v>
       </c>
       <c r="F121" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="G121" s="3" t="s">
         <v>332</v>
-      </c>
-      <c r="G121" s="3" t="s">
-        <v>333</v>
       </c>
       <c r="H121" s="3">
         <v>0</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K121" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L121" s="3"/>
     </row>

</xml_diff>